<commit_message>
Added scores table data
</commit_message>
<xml_diff>
--- a/uBetCha/uploads/Scores.xlsx
+++ b/uBetCha/uploads/Scores.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\School\IS 4880 - Capstone\ISCapstone\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\School\IS 4880 - Capstone\ISCapstone\uBetCha\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC9B2989-C7F4-4CF2-B5A6-EE3A4F0CFFDE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{70FBD382-572A-4AAE-B6E4-2E37433462A9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Scores" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -736,7 +736,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -746,9 +746,6 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1108,10 +1105,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H169"/>
+  <dimension ref="A1:G169"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1122,10 +1119,9 @@
     <col min="5" max="5" width="6" customWidth="1"/>
     <col min="6" max="6" width="23.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.7109375" customWidth="1"/>
-    <col min="8" max="8" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>45</v>
       </c>
@@ -1148,11 +1144,11 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>51</v>
       </c>
       <c r="C2" s="2" t="s">
@@ -1170,14 +1166,13 @@
       <c r="G2" s="2">
         <v>118</v>
       </c>
-      <c r="H2" s="4"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>51</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -1195,14 +1190,13 @@
       <c r="G3" s="2">
         <v>85</v>
       </c>
-      <c r="H3" s="4"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ref="A4:A67" si="0">A3+1</f>
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>51</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -1220,14 +1214,13 @@
       <c r="G4" s="2">
         <v>89</v>
       </c>
-      <c r="H4" s="4"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>51</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -1245,14 +1238,13 @@
       <c r="G5" s="2">
         <v>112</v>
       </c>
-      <c r="H5" s="4"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>51</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -1270,14 +1262,13 @@
       <c r="G6" s="2">
         <v>113</v>
       </c>
-      <c r="H6" s="4"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>51</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -1295,14 +1286,13 @@
       <c r="G7" s="2">
         <v>116</v>
       </c>
-      <c r="H7" s="4"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>51</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -1320,14 +1310,13 @@
       <c r="G8" s="2">
         <v>123</v>
       </c>
-      <c r="H8" s="4"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>51</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -1345,14 +1334,13 @@
       <c r="G9" s="2">
         <v>114</v>
       </c>
-      <c r="H9" s="4"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>51</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -1370,14 +1358,13 @@
       <c r="G10" s="2">
         <v>113</v>
       </c>
-      <c r="H10" s="4"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>51</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -1395,14 +1382,13 @@
       <c r="G11" s="2">
         <v>124</v>
       </c>
-      <c r="H11" s="4"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>52</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -1420,14 +1406,13 @@
       <c r="G12" s="2">
         <v>128</v>
       </c>
-      <c r="H12" s="4"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>52</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -1445,14 +1430,13 @@
       <c r="G13" s="2">
         <v>117</v>
       </c>
-      <c r="H13" s="4"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="4" t="s">
         <v>52</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -1470,14 +1454,13 @@
       <c r="G14" s="2">
         <v>129</v>
       </c>
-      <c r="H14" s="4"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="4" t="s">
         <v>52</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -1495,14 +1478,13 @@
       <c r="G15" s="2">
         <v>129</v>
       </c>
-      <c r="H15" s="4"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="4" t="s">
         <v>53</v>
       </c>
       <c r="C16" s="2" t="s">
@@ -1520,14 +1502,13 @@
       <c r="G16" s="2">
         <v>100</v>
       </c>
-      <c r="H16" s="4"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="4" t="s">
         <v>53</v>
       </c>
       <c r="C17" s="2" t="s">
@@ -1545,14 +1526,13 @@
       <c r="G17" s="2">
         <v>134</v>
       </c>
-      <c r="H17" s="4"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="4" t="s">
         <v>53</v>
       </c>
       <c r="C18" s="2" t="s">
@@ -1570,14 +1550,13 @@
       <c r="G18" s="2">
         <v>103</v>
       </c>
-      <c r="H18" s="4"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="4" t="s">
         <v>53</v>
       </c>
       <c r="C19" s="2" t="s">
@@ -1595,14 +1574,13 @@
       <c r="G19" s="2">
         <v>117</v>
       </c>
-      <c r="H19" s="4"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="4" t="s">
         <v>53</v>
       </c>
       <c r="C20" s="2" t="s">
@@ -1620,14 +1598,13 @@
       <c r="G20" s="2">
         <v>115</v>
       </c>
-      <c r="H20" s="4"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="4" t="s">
         <v>53</v>
       </c>
       <c r="C21" s="2" t="s">
@@ -1645,14 +1622,13 @@
       <c r="G21" s="2">
         <v>119</v>
       </c>
-      <c r="H21" s="4"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="4" t="s">
         <v>53</v>
       </c>
       <c r="C22" s="2" t="s">
@@ -1670,14 +1646,13 @@
       <c r="G22" s="2">
         <v>137</v>
       </c>
-      <c r="H22" s="4"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="4" t="s">
         <v>53</v>
       </c>
       <c r="C23" s="2" t="s">
@@ -1695,14 +1670,13 @@
       <c r="G23" s="2">
         <v>96</v>
       </c>
-      <c r="H23" s="4"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="4" t="s">
         <v>53</v>
       </c>
       <c r="C24" s="2" t="s">
@@ -1720,14 +1694,13 @@
       <c r="G24" s="2">
         <v>113</v>
       </c>
-      <c r="H24" s="4"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="4" t="s">
         <v>53</v>
       </c>
       <c r="C25" s="2" t="s">
@@ -1745,14 +1718,13 @@
       <c r="G25" s="2">
         <v>108</v>
       </c>
-      <c r="H25" s="4"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="4" t="s">
         <v>54</v>
       </c>
       <c r="C26" s="2" t="s">
@@ -1770,14 +1742,13 @@
       <c r="G26" s="2">
         <v>108</v>
       </c>
-      <c r="H26" s="4"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="4" t="s">
         <v>54</v>
       </c>
       <c r="C27" s="2" t="s">
@@ -1795,14 +1766,13 @@
       <c r="G27" s="2">
         <v>125</v>
       </c>
-      <c r="H27" s="4"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="4" t="s">
         <v>54</v>
       </c>
       <c r="C28" s="2" t="s">
@@ -1820,14 +1790,13 @@
       <c r="G28" s="2">
         <v>127</v>
       </c>
-      <c r="H28" s="4"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="4" t="s">
         <v>54</v>
       </c>
       <c r="C29" s="2" t="s">
@@ -1845,14 +1814,13 @@
       <c r="G29" s="2">
         <v>129</v>
       </c>
-      <c r="H29" s="4"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="4" t="s">
         <v>55</v>
       </c>
       <c r="C30" s="2" t="s">
@@ -1870,14 +1838,13 @@
       <c r="G30" s="2">
         <v>116</v>
       </c>
-      <c r="H30" s="4"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="4" t="s">
         <v>55</v>
       </c>
       <c r="C31" s="2" t="s">
@@ -1895,14 +1862,13 @@
       <c r="G31" s="2">
         <v>116</v>
       </c>
-      <c r="H31" s="4"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="4" t="s">
         <v>55</v>
       </c>
       <c r="C32" s="2" t="s">
@@ -1920,14 +1886,13 @@
       <c r="G32" s="2">
         <v>129</v>
       </c>
-      <c r="H32" s="4"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="4" t="s">
         <v>55</v>
       </c>
       <c r="C33" s="2" t="s">
@@ -1945,14 +1910,13 @@
       <c r="G33" s="2">
         <v>119</v>
       </c>
-      <c r="H33" s="4"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="4" t="s">
         <v>55</v>
       </c>
       <c r="C34" s="2" t="s">
@@ -1970,14 +1934,13 @@
       <c r="G34" s="2">
         <v>120</v>
       </c>
-      <c r="H34" s="4"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="4" t="s">
         <v>55</v>
       </c>
       <c r="C35" s="2" t="s">
@@ -1995,14 +1958,13 @@
       <c r="G35" s="2">
         <v>109</v>
       </c>
-      <c r="H35" s="4"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B36" s="4" t="s">
         <v>55</v>
       </c>
       <c r="C36" s="2" t="s">
@@ -2020,14 +1982,13 @@
       <c r="G36" s="2">
         <v>107</v>
       </c>
-      <c r="H36" s="4"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B37" s="4" t="s">
         <v>55</v>
       </c>
       <c r="C37" s="2" t="s">
@@ -2045,14 +2006,13 @@
       <c r="G37" s="2">
         <v>95</v>
       </c>
-      <c r="H37" s="4"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="4" t="s">
         <v>55</v>
       </c>
       <c r="C38" s="2" t="s">
@@ -2070,14 +2030,13 @@
       <c r="G38" s="2">
         <v>128</v>
       </c>
-      <c r="H38" s="4"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B39" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C39" s="2" t="s">
@@ -2095,14 +2054,13 @@
       <c r="G39" s="2">
         <v>105</v>
       </c>
-      <c r="H39" s="4"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B40" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C40" s="2" t="s">
@@ -2120,14 +2078,13 @@
       <c r="G40" s="2">
         <v>119</v>
       </c>
-      <c r="H40" s="4"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B41" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C41" s="2" t="s">
@@ -2145,14 +2102,13 @@
       <c r="G41" s="2">
         <v>112</v>
       </c>
-      <c r="H41" s="4"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B42" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C42" s="2" t="s">
@@ -2170,14 +2126,13 @@
       <c r="G42" s="2">
         <v>125</v>
       </c>
-      <c r="H42" s="4"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="B43" s="4" t="s">
         <v>56</v>
       </c>
       <c r="C43" s="2" t="s">
@@ -2195,14 +2150,13 @@
       <c r="G43" s="2">
         <v>111</v>
       </c>
-      <c r="H43" s="4"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="B44" s="4" t="s">
         <v>57</v>
       </c>
       <c r="C44" s="2" t="s">
@@ -2220,14 +2174,13 @@
       <c r="G44" s="2">
         <v>119</v>
       </c>
-      <c r="H44" s="4"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="B45" s="4" t="s">
         <v>57</v>
       </c>
       <c r="C45" s="2" t="s">
@@ -2245,14 +2198,13 @@
       <c r="G45" s="2">
         <v>119</v>
       </c>
-      <c r="H45" s="4"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B46" s="4" t="s">
         <v>57</v>
       </c>
       <c r="C46" s="2" t="s">
@@ -2270,14 +2222,13 @@
       <c r="G46" s="2">
         <v>112</v>
       </c>
-      <c r="H46" s="4"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47">
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B47" s="4" t="s">
         <v>57</v>
       </c>
       <c r="C47" s="2" t="s">
@@ -2295,14 +2246,13 @@
       <c r="G47" s="2">
         <v>106</v>
       </c>
-      <c r="H47" s="4"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48">
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B48" s="4" t="s">
         <v>57</v>
       </c>
       <c r="C48" s="2" t="s">
@@ -2320,14 +2270,13 @@
       <c r="G48" s="2">
         <v>108</v>
       </c>
-      <c r="H48" s="4"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="B49" s="4" t="s">
         <v>57</v>
       </c>
       <c r="C49" s="2" t="s">
@@ -2345,14 +2294,13 @@
       <c r="G49" s="2">
         <v>127</v>
       </c>
-      <c r="H49" s="4"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
-      <c r="B50" s="5" t="s">
+      <c r="B50" s="4" t="s">
         <v>57</v>
       </c>
       <c r="C50" s="2" t="s">
@@ -2370,14 +2318,13 @@
       <c r="G50" s="2">
         <v>105</v>
       </c>
-      <c r="H50" s="4"/>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="B51" s="5" t="s">
+      <c r="B51" s="4" t="s">
         <v>57</v>
       </c>
       <c r="C51" s="2" t="s">
@@ -2395,14 +2342,13 @@
       <c r="G51" s="2">
         <v>117</v>
       </c>
-      <c r="H51" s="4"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52">
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
-      <c r="B52" s="5" t="s">
+      <c r="B52" s="4" t="s">
         <v>58</v>
       </c>
       <c r="C52" s="2" t="s">
@@ -2420,14 +2366,13 @@
       <c r="G52" s="2">
         <v>95</v>
       </c>
-      <c r="H52" s="4"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53">
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
-      <c r="B53" s="5" t="s">
+      <c r="B53" s="4" t="s">
         <v>58</v>
       </c>
       <c r="C53" s="2" t="s">
@@ -2445,14 +2390,13 @@
       <c r="G53" s="2">
         <v>100</v>
       </c>
-      <c r="H53" s="4"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54">
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
-      <c r="B54" s="5" t="s">
+      <c r="B54" s="4" t="s">
         <v>58</v>
       </c>
       <c r="C54" s="2" t="s">
@@ -2470,14 +2414,13 @@
       <c r="G54" s="2">
         <v>92</v>
       </c>
-      <c r="H54" s="4"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55">
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
-      <c r="B55" s="5" t="s">
+      <c r="B55" s="4" t="s">
         <v>58</v>
       </c>
       <c r="C55" s="2" t="s">
@@ -2495,14 +2438,13 @@
       <c r="G55" s="2">
         <v>117</v>
       </c>
-      <c r="H55" s="4"/>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
-      <c r="B56" s="5" t="s">
+      <c r="B56" s="4" t="s">
         <v>58</v>
       </c>
       <c r="C56" s="2" t="s">
@@ -2520,14 +2462,13 @@
       <c r="G56" s="2">
         <v>119</v>
       </c>
-      <c r="H56" s="4"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57">
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
-      <c r="B57" s="5" t="s">
+      <c r="B57" s="4" t="s">
         <v>58</v>
       </c>
       <c r="C57" s="2" t="s">
@@ -2545,14 +2486,13 @@
       <c r="G57" s="2">
         <v>142</v>
       </c>
-      <c r="H57" s="4"/>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58">
         <f t="shared" si="0"/>
         <v>57</v>
       </c>
-      <c r="B58" s="5" t="s">
+      <c r="B58" s="4" t="s">
         <v>58</v>
       </c>
       <c r="C58" s="2" t="s">
@@ -2570,14 +2510,13 @@
       <c r="G58" s="2">
         <v>120</v>
       </c>
-      <c r="H58" s="4"/>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59">
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
-      <c r="B59" s="5" t="s">
+      <c r="B59" s="4" t="s">
         <v>58</v>
       </c>
       <c r="C59" s="2" t="s">
@@ -2595,14 +2534,13 @@
       <c r="G59" s="2">
         <v>108</v>
       </c>
-      <c r="H59" s="4"/>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60">
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
-      <c r="B60" s="5" t="s">
+      <c r="B60" s="4" t="s">
         <v>58</v>
       </c>
       <c r="C60" s="2" t="s">
@@ -2620,14 +2558,13 @@
       <c r="G60" s="2">
         <v>122</v>
       </c>
-      <c r="H60" s="4"/>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="B61" s="5" t="s">
+      <c r="B61" s="4" t="s">
         <v>59</v>
       </c>
       <c r="C61" s="2" t="s">
@@ -2645,14 +2582,13 @@
       <c r="G61" s="2">
         <v>111</v>
       </c>
-      <c r="H61" s="4"/>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62">
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
-      <c r="B62" s="5" t="s">
+      <c r="B62" s="4" t="s">
         <v>59</v>
       </c>
       <c r="C62" s="2" t="s">
@@ -2670,14 +2606,13 @@
       <c r="G62" s="2">
         <v>140</v>
       </c>
-      <c r="H62" s="4"/>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63">
         <f t="shared" si="0"/>
         <v>62</v>
       </c>
-      <c r="B63" s="5" t="s">
+      <c r="B63" s="4" t="s">
         <v>59</v>
       </c>
       <c r="C63" s="2" t="s">
@@ -2695,14 +2630,13 @@
       <c r="G63" s="2">
         <v>118</v>
       </c>
-      <c r="H63" s="4"/>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64">
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
-      <c r="B64" s="5" t="s">
+      <c r="B64" s="4" t="s">
         <v>59</v>
       </c>
       <c r="C64" s="2" t="s">
@@ -2720,14 +2654,13 @@
       <c r="G64" s="2">
         <v>99</v>
       </c>
-      <c r="H64" s="4"/>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65">
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
-      <c r="B65" s="5" t="s">
+      <c r="B65" s="4" t="s">
         <v>59</v>
       </c>
       <c r="C65" s="2" t="s">
@@ -2745,14 +2678,13 @@
       <c r="G65" s="2">
         <v>113</v>
       </c>
-      <c r="H65" s="4"/>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66">
         <f t="shared" si="0"/>
         <v>65</v>
       </c>
-      <c r="B66" s="5" t="s">
+      <c r="B66" s="4" t="s">
         <v>59</v>
       </c>
       <c r="C66" s="2" t="s">
@@ -2770,14 +2702,13 @@
       <c r="G66" s="2">
         <v>92</v>
       </c>
-      <c r="H66" s="4"/>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67">
         <f t="shared" si="0"/>
         <v>66</v>
       </c>
-      <c r="B67" s="5" t="s">
+      <c r="B67" s="4" t="s">
         <v>59</v>
       </c>
       <c r="C67" s="2" t="s">
@@ -2795,14 +2726,13 @@
       <c r="G67" s="2">
         <v>115</v>
       </c>
-      <c r="H67" s="4"/>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68">
         <f t="shared" ref="A68:A131" si="1">A67+1</f>
         <v>67</v>
       </c>
-      <c r="B68" s="5" t="s">
+      <c r="B68" s="4" t="s">
         <v>60</v>
       </c>
       <c r="C68" s="2" t="s">
@@ -2820,14 +2750,13 @@
       <c r="G68" s="2">
         <v>76</v>
       </c>
-      <c r="H68" s="4"/>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69">
         <f t="shared" si="1"/>
         <v>68</v>
       </c>
-      <c r="B69" s="5" t="s">
+      <c r="B69" s="4" t="s">
         <v>60</v>
       </c>
       <c r="C69" s="2" t="s">
@@ -2845,14 +2774,13 @@
       <c r="G69" s="2">
         <v>105</v>
       </c>
-      <c r="H69" s="4"/>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70">
         <f t="shared" si="1"/>
         <v>69</v>
       </c>
-      <c r="B70" s="5" t="s">
+      <c r="B70" s="4" t="s">
         <v>60</v>
       </c>
       <c r="C70" s="2" t="s">
@@ -2870,14 +2798,13 @@
       <c r="G70" s="2">
         <v>135</v>
       </c>
-      <c r="H70" s="4"/>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71">
         <f t="shared" si="1"/>
         <v>70</v>
       </c>
-      <c r="B71" s="5" t="s">
+      <c r="B71" s="4" t="s">
         <v>60</v>
       </c>
       <c r="C71" s="2" t="s">
@@ -2895,14 +2822,13 @@
       <c r="G71" s="2">
         <v>137</v>
       </c>
-      <c r="H71" s="4"/>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72">
         <f t="shared" si="1"/>
         <v>71</v>
       </c>
-      <c r="B72" s="5" t="s">
+      <c r="B72" s="4" t="s">
         <v>60</v>
       </c>
       <c r="C72" s="2" t="s">
@@ -2920,14 +2846,13 @@
       <c r="G72" s="2">
         <v>123</v>
       </c>
-      <c r="H72" s="4"/>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73">
         <f t="shared" si="1"/>
         <v>72</v>
       </c>
-      <c r="B73" s="5" t="s">
+      <c r="B73" s="4" t="s">
         <v>60</v>
       </c>
       <c r="C73" s="2" t="s">
@@ -2945,14 +2870,13 @@
       <c r="G73" s="2">
         <v>119</v>
       </c>
-      <c r="H73" s="4"/>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74">
         <f t="shared" si="1"/>
         <v>73</v>
       </c>
-      <c r="B74" s="5" t="s">
+      <c r="B74" s="4" t="s">
         <v>60</v>
       </c>
       <c r="C74" s="2" t="s">
@@ -2970,14 +2894,13 @@
       <c r="G74" s="2">
         <v>127</v>
       </c>
-      <c r="H74" s="4"/>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75">
         <f t="shared" si="1"/>
         <v>74</v>
       </c>
-      <c r="B75" s="5" t="s">
+      <c r="B75" s="4" t="s">
         <v>60</v>
       </c>
       <c r="C75" s="2" t="s">
@@ -2995,14 +2918,13 @@
       <c r="G75" s="2">
         <v>101</v>
       </c>
-      <c r="H75" s="4"/>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76">
         <f t="shared" si="1"/>
         <v>75</v>
       </c>
-      <c r="B76" s="5" t="s">
+      <c r="B76" s="4" t="s">
         <v>60</v>
       </c>
       <c r="C76" s="2" t="s">
@@ -3020,14 +2942,13 @@
       <c r="G76" s="2">
         <v>125</v>
       </c>
-      <c r="H76" s="4"/>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77">
         <f t="shared" si="1"/>
         <v>76</v>
       </c>
-      <c r="B77" s="5" t="s">
+      <c r="B77" s="4" t="s">
         <v>61</v>
       </c>
       <c r="C77" s="2" t="s">
@@ -3045,14 +2966,13 @@
       <c r="G77" s="2">
         <v>110</v>
       </c>
-      <c r="H77" s="4"/>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78">
         <f t="shared" si="1"/>
         <v>77</v>
       </c>
-      <c r="B78" s="5" t="s">
+      <c r="B78" s="4" t="s">
         <v>61</v>
       </c>
       <c r="C78" s="2" t="s">
@@ -3070,14 +2990,13 @@
       <c r="G78" s="2">
         <v>126</v>
       </c>
-      <c r="H78" s="4"/>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79">
         <f t="shared" si="1"/>
         <v>78</v>
       </c>
-      <c r="B79" s="5" t="s">
+      <c r="B79" s="4" t="s">
         <v>61</v>
       </c>
       <c r="C79" s="2" t="s">
@@ -3095,14 +3014,13 @@
       <c r="G79" s="2">
         <v>138</v>
       </c>
-      <c r="H79" s="4"/>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80">
         <f t="shared" si="1"/>
         <v>79</v>
       </c>
-      <c r="B80" s="5" t="s">
+      <c r="B80" s="4" t="s">
         <v>61</v>
       </c>
       <c r="C80" s="2" t="s">
@@ -3120,14 +3038,13 @@
       <c r="G80" s="2">
         <v>106</v>
       </c>
-      <c r="H80" s="4"/>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81">
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
-      <c r="B81" s="5" t="s">
+      <c r="B81" s="4" t="s">
         <v>61</v>
       </c>
       <c r="C81" s="2" t="s">
@@ -3145,14 +3062,13 @@
       <c r="G81" s="2">
         <v>116</v>
       </c>
-      <c r="H81" s="4"/>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82">
         <f t="shared" si="1"/>
         <v>81</v>
       </c>
-      <c r="B82" s="5" t="s">
+      <c r="B82" s="4" t="s">
         <v>62</v>
       </c>
       <c r="C82" s="2" t="s">
@@ -3170,14 +3086,13 @@
       <c r="G82" s="2">
         <v>127</v>
       </c>
-      <c r="H82" s="4"/>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83">
         <f t="shared" si="1"/>
         <v>82</v>
       </c>
-      <c r="B83" s="5" t="s">
+      <c r="B83" s="4" t="s">
         <v>62</v>
       </c>
       <c r="C83" s="2" t="s">
@@ -3195,14 +3110,13 @@
       <c r="G83" s="2">
         <v>116</v>
       </c>
-      <c r="H83" s="4"/>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84">
         <f t="shared" si="1"/>
         <v>83</v>
       </c>
-      <c r="B84" s="5" t="s">
+      <c r="B84" s="4" t="s">
         <v>62</v>
       </c>
       <c r="C84" s="2" t="s">
@@ -3220,14 +3134,13 @@
       <c r="G84" s="2">
         <v>101</v>
       </c>
-      <c r="H84" s="4"/>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85">
         <f t="shared" si="1"/>
         <v>84</v>
       </c>
-      <c r="B85" s="5" t="s">
+      <c r="B85" s="4" t="s">
         <v>62</v>
       </c>
       <c r="C85" s="2" t="s">
@@ -3245,14 +3158,13 @@
       <c r="G85" s="2">
         <v>118</v>
       </c>
-      <c r="H85" s="4"/>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86">
         <f t="shared" si="1"/>
         <v>85</v>
       </c>
-      <c r="B86" s="5" t="s">
+      <c r="B86" s="4" t="s">
         <v>62</v>
       </c>
       <c r="C86" s="2" t="s">
@@ -3270,14 +3182,13 @@
       <c r="G86" s="2">
         <v>96</v>
       </c>
-      <c r="H86" s="4"/>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87">
         <f t="shared" si="1"/>
         <v>86</v>
       </c>
-      <c r="B87" s="5" t="s">
+      <c r="B87" s="4" t="s">
         <v>62</v>
       </c>
       <c r="C87" s="2" t="s">
@@ -3295,14 +3206,13 @@
       <c r="G87" s="2">
         <v>111</v>
       </c>
-      <c r="H87" s="4"/>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88">
         <f t="shared" si="1"/>
         <v>87</v>
       </c>
-      <c r="B88" s="5" t="s">
+      <c r="B88" s="4" t="s">
         <v>62</v>
       </c>
       <c r="C88" s="2" t="s">
@@ -3320,14 +3230,13 @@
       <c r="G88" s="2">
         <v>108</v>
       </c>
-      <c r="H88" s="4"/>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89">
         <f t="shared" si="1"/>
         <v>88</v>
       </c>
-      <c r="B89" s="5" t="s">
+      <c r="B89" s="4" t="s">
         <v>62</v>
       </c>
       <c r="C89" s="2" t="s">
@@ -3345,14 +3254,13 @@
       <c r="G89" s="2">
         <v>130</v>
       </c>
-      <c r="H89" s="4"/>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90">
         <f t="shared" si="1"/>
         <v>89</v>
       </c>
-      <c r="B90" s="5" t="s">
+      <c r="B90" s="4" t="s">
         <v>62</v>
       </c>
       <c r="C90" s="2" t="s">
@@ -3370,14 +3278,13 @@
       <c r="G90" s="2">
         <v>112</v>
       </c>
-      <c r="H90" s="4"/>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91">
         <f t="shared" si="1"/>
         <v>90</v>
       </c>
-      <c r="B91" s="5" t="s">
+      <c r="B91" s="4" t="s">
         <v>62</v>
       </c>
       <c r="C91" s="2" t="s">
@@ -3395,14 +3302,13 @@
       <c r="G91" s="2">
         <v>116</v>
       </c>
-      <c r="H91" s="4"/>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92">
         <f t="shared" si="1"/>
         <v>91</v>
       </c>
-      <c r="B92" s="5" t="s">
+      <c r="B92" s="4" t="s">
         <v>62</v>
       </c>
       <c r="C92" s="2" t="s">
@@ -3420,14 +3326,13 @@
       <c r="G92" s="2">
         <v>116</v>
       </c>
-      <c r="H92" s="4"/>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93">
         <f t="shared" si="1"/>
         <v>92</v>
       </c>
-      <c r="B93" s="5" t="s">
+      <c r="B93" s="4" t="s">
         <v>63</v>
       </c>
       <c r="C93" s="2" t="s">
@@ -3445,14 +3350,13 @@
       <c r="G93" s="2">
         <v>141</v>
       </c>
-      <c r="H93" s="4"/>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94">
         <f t="shared" si="1"/>
         <v>93</v>
       </c>
-      <c r="B94" s="5" t="s">
+      <c r="B94" s="4" t="s">
         <v>63</v>
       </c>
       <c r="C94" s="2" t="s">
@@ -3470,14 +3374,13 @@
       <c r="G94" s="2">
         <v>118</v>
       </c>
-      <c r="H94" s="4"/>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95">
         <f t="shared" si="1"/>
         <v>94</v>
       </c>
-      <c r="B95" s="5" t="s">
+      <c r="B95" s="4" t="s">
         <v>64</v>
       </c>
       <c r="C95" s="2" t="s">
@@ -3495,14 +3398,13 @@
       <c r="G95" s="2">
         <v>106</v>
       </c>
-      <c r="H95" s="4"/>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96">
         <f t="shared" si="1"/>
         <v>95</v>
       </c>
-      <c r="B96" s="5" t="s">
+      <c r="B96" s="4" t="s">
         <v>64</v>
       </c>
       <c r="C96" s="2" t="s">
@@ -3520,14 +3422,13 @@
       <c r="G96" s="2">
         <v>129</v>
       </c>
-      <c r="H96" s="4"/>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97">
         <f t="shared" si="1"/>
         <v>96</v>
       </c>
-      <c r="B97" s="5" t="s">
+      <c r="B97" s="4" t="s">
         <v>64</v>
       </c>
       <c r="C97" s="2" t="s">
@@ -3545,14 +3446,13 @@
       <c r="G97" s="2">
         <v>93</v>
       </c>
-      <c r="H97" s="4"/>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98">
         <f t="shared" si="1"/>
         <v>97</v>
       </c>
-      <c r="B98" s="5" t="s">
+      <c r="B98" s="4" t="s">
         <v>64</v>
       </c>
       <c r="C98" s="2" t="s">
@@ -3570,14 +3470,13 @@
       <c r="G98" s="2">
         <v>112</v>
       </c>
-      <c r="H98" s="4"/>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99">
         <f t="shared" si="1"/>
         <v>98</v>
       </c>
-      <c r="B99" s="5" t="s">
+      <c r="B99" s="4" t="s">
         <v>64</v>
       </c>
       <c r="C99" s="2" t="s">
@@ -3595,14 +3494,13 @@
       <c r="G99" s="2">
         <v>129</v>
       </c>
-      <c r="H99" s="4"/>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100">
         <f t="shared" si="1"/>
         <v>99</v>
       </c>
-      <c r="B100" s="5" t="s">
+      <c r="B100" s="4" t="s">
         <v>64</v>
       </c>
       <c r="C100" s="2" t="s">
@@ -3620,14 +3518,13 @@
       <c r="G100" s="2">
         <v>105</v>
       </c>
-      <c r="H100" s="4"/>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="B101" s="5" t="s">
+      <c r="B101" s="4" t="s">
         <v>65</v>
       </c>
       <c r="C101" s="2" t="s">
@@ -3645,14 +3542,13 @@
       <c r="G101" s="2">
         <v>106</v>
       </c>
-      <c r="H101" s="4"/>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102">
         <f t="shared" si="1"/>
         <v>101</v>
       </c>
-      <c r="B102" s="5" t="s">
+      <c r="B102" s="4" t="s">
         <v>65</v>
       </c>
       <c r="C102" s="2" t="s">
@@ -3670,14 +3566,13 @@
       <c r="G102" s="2">
         <v>108</v>
       </c>
-      <c r="H102" s="4"/>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103">
         <f t="shared" si="1"/>
         <v>102</v>
       </c>
-      <c r="B103" s="5" t="s">
+      <c r="B103" s="4" t="s">
         <v>65</v>
       </c>
       <c r="C103" s="2" t="s">
@@ -3695,14 +3590,13 @@
       <c r="G103" s="2">
         <v>98</v>
       </c>
-      <c r="H103" s="4"/>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104">
         <f t="shared" si="1"/>
         <v>103</v>
       </c>
-      <c r="B104" s="5" t="s">
+      <c r="B104" s="4" t="s">
         <v>65</v>
       </c>
       <c r="C104" s="2" t="s">
@@ -3720,14 +3614,13 @@
       <c r="G104" s="2">
         <v>118</v>
       </c>
-      <c r="H104" s="4"/>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105">
         <f t="shared" si="1"/>
         <v>104</v>
       </c>
-      <c r="B105" s="5" t="s">
+      <c r="B105" s="4" t="s">
         <v>65</v>
       </c>
       <c r="C105" s="2" t="s">
@@ -3745,14 +3638,13 @@
       <c r="G105" s="2">
         <v>117</v>
       </c>
-      <c r="H105" s="4"/>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106">
         <f t="shared" si="1"/>
         <v>105</v>
       </c>
-      <c r="B106" s="5" t="s">
+      <c r="B106" s="4" t="s">
         <v>65</v>
       </c>
       <c r="C106" s="2" t="s">
@@ -3770,14 +3662,13 @@
       <c r="G106" s="2">
         <v>113</v>
       </c>
-      <c r="H106" s="4"/>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107">
         <f t="shared" si="1"/>
         <v>106</v>
       </c>
-      <c r="B107" s="5" t="s">
+      <c r="B107" s="4" t="s">
         <v>65</v>
       </c>
       <c r="C107" s="2" t="s">
@@ -3795,14 +3686,13 @@
       <c r="G107" s="2">
         <v>104</v>
       </c>
-      <c r="H107" s="4"/>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108">
         <f t="shared" si="1"/>
         <v>107</v>
       </c>
-      <c r="B108" s="5" t="s">
+      <c r="B108" s="4" t="s">
         <v>65</v>
       </c>
       <c r="C108" s="2" t="s">
@@ -3820,14 +3710,13 @@
       <c r="G108" s="2">
         <v>117</v>
       </c>
-      <c r="H108" s="4"/>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109">
         <f t="shared" si="1"/>
         <v>108</v>
       </c>
-      <c r="B109" s="5" t="s">
+      <c r="B109" s="4" t="s">
         <v>65</v>
       </c>
       <c r="C109" s="2" t="s">
@@ -3845,14 +3734,13 @@
       <c r="G109" s="2">
         <v>115</v>
       </c>
-      <c r="H109" s="4"/>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110">
         <f t="shared" si="1"/>
         <v>109</v>
       </c>
-      <c r="B110" s="5" t="s">
+      <c r="B110" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C110" s="2" t="s">
@@ -3870,14 +3758,13 @@
       <c r="G110" s="2">
         <v>103</v>
       </c>
-      <c r="H110" s="4"/>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111">
         <f t="shared" si="1"/>
         <v>110</v>
       </c>
-      <c r="B111" s="5" t="s">
+      <c r="B111" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C111" s="2" t="s">
@@ -3895,14 +3782,13 @@
       <c r="G111" s="2">
         <v>86</v>
       </c>
-      <c r="H111" s="4"/>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112">
         <f t="shared" si="1"/>
         <v>111</v>
       </c>
-      <c r="B112" s="5" t="s">
+      <c r="B112" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C112" s="2" t="s">
@@ -3920,14 +3806,13 @@
       <c r="G112" s="2">
         <v>111</v>
       </c>
-      <c r="H112" s="4"/>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113">
         <f t="shared" si="1"/>
         <v>112</v>
       </c>
-      <c r="B113" s="5" t="s">
+      <c r="B113" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C113" s="2" t="s">
@@ -3945,14 +3830,13 @@
       <c r="G113" s="2">
         <v>104</v>
       </c>
-      <c r="H113" s="4"/>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114">
         <f t="shared" si="1"/>
         <v>113</v>
       </c>
-      <c r="B114" s="5" t="s">
+      <c r="B114" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C114" s="2" t="s">
@@ -3970,14 +3854,13 @@
       <c r="G114" s="2">
         <v>124</v>
       </c>
-      <c r="H114" s="4"/>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115">
         <f t="shared" si="1"/>
         <v>114</v>
       </c>
-      <c r="B115" s="5" t="s">
+      <c r="B115" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C115" s="2" t="s">
@@ -3995,14 +3878,13 @@
       <c r="G115" s="2">
         <v>119</v>
       </c>
-      <c r="H115" s="4"/>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116">
         <f t="shared" si="1"/>
         <v>115</v>
       </c>
-      <c r="B116" s="5" t="s">
+      <c r="B116" s="4" t="s">
         <v>66</v>
       </c>
       <c r="C116" s="2" t="s">
@@ -4020,14 +3902,13 @@
       <c r="G116" s="2">
         <v>110</v>
       </c>
-      <c r="H116" s="4"/>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117">
         <f t="shared" si="1"/>
         <v>116</v>
       </c>
-      <c r="B117" s="5" t="s">
+      <c r="B117" s="4" t="s">
         <v>67</v>
       </c>
       <c r="C117" s="2" t="s">
@@ -4045,14 +3926,13 @@
       <c r="G117" s="2">
         <v>114</v>
       </c>
-      <c r="H117" s="4"/>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118">
         <f t="shared" si="1"/>
         <v>117</v>
       </c>
-      <c r="B118" s="5" t="s">
+      <c r="B118" s="4" t="s">
         <v>67</v>
       </c>
       <c r="C118" s="2" t="s">
@@ -4070,14 +3950,13 @@
       <c r="G118" s="2">
         <v>128</v>
       </c>
-      <c r="H118" s="4"/>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119">
         <f t="shared" si="1"/>
         <v>118</v>
       </c>
-      <c r="B119" s="5" t="s">
+      <c r="B119" s="4" t="s">
         <v>67</v>
       </c>
       <c r="C119" s="2" t="s">
@@ -4095,14 +3974,13 @@
       <c r="G119" s="2">
         <v>127</v>
       </c>
-      <c r="H119" s="4"/>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120">
         <f t="shared" si="1"/>
         <v>119</v>
       </c>
-      <c r="B120" s="5" t="s">
+      <c r="B120" s="4" t="s">
         <v>67</v>
       </c>
       <c r="C120" s="2" t="s">
@@ -4120,14 +3998,13 @@
       <c r="G120" s="2">
         <v>126</v>
       </c>
-      <c r="H120" s="4"/>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121">
         <f t="shared" si="1"/>
         <v>120</v>
       </c>
-      <c r="B121" s="5" t="s">
+      <c r="B121" s="4" t="s">
         <v>67</v>
       </c>
       <c r="C121" s="2" t="s">
@@ -4145,14 +4022,13 @@
       <c r="G121" s="2">
         <v>131</v>
       </c>
-      <c r="H121" s="4"/>
-    </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122">
         <f t="shared" si="1"/>
         <v>121</v>
       </c>
-      <c r="B122" s="5" t="s">
+      <c r="B122" s="4" t="s">
         <v>67</v>
       </c>
       <c r="C122" s="2" t="s">
@@ -4170,14 +4046,13 @@
       <c r="G122" s="2">
         <v>101</v>
       </c>
-      <c r="H122" s="4"/>
-    </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123">
         <f t="shared" si="1"/>
         <v>122</v>
       </c>
-      <c r="B123" s="5" t="s">
+      <c r="B123" s="4" t="s">
         <v>67</v>
       </c>
       <c r="C123" s="2" t="s">
@@ -4195,14 +4070,13 @@
       <c r="G123" s="2">
         <v>107</v>
       </c>
-      <c r="H123" s="4"/>
-    </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124">
         <f t="shared" si="1"/>
         <v>123</v>
       </c>
-      <c r="B124" s="5" t="s">
+      <c r="B124" s="4" t="s">
         <v>68</v>
       </c>
       <c r="C124" s="2" t="s">
@@ -4220,14 +4094,13 @@
       <c r="G124" s="2">
         <v>125</v>
       </c>
-      <c r="H124" s="4"/>
-    </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125">
         <f t="shared" si="1"/>
         <v>124</v>
       </c>
-      <c r="B125" s="5" t="s">
+      <c r="B125" s="4" t="s">
         <v>68</v>
       </c>
       <c r="C125" s="2" t="s">
@@ -4245,14 +4118,13 @@
       <c r="G125" s="2">
         <v>129</v>
       </c>
-      <c r="H125" s="4"/>
-    </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126">
         <f t="shared" si="1"/>
         <v>125</v>
       </c>
-      <c r="B126" s="5" t="s">
+      <c r="B126" s="4" t="s">
         <v>68</v>
       </c>
       <c r="C126" s="2" t="s">
@@ -4270,14 +4142,13 @@
       <c r="G126" s="2">
         <v>134</v>
       </c>
-      <c r="H126" s="4"/>
-    </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127">
         <f t="shared" si="1"/>
         <v>126</v>
       </c>
-      <c r="B127" s="5" t="s">
+      <c r="B127" s="4" t="s">
         <v>68</v>
       </c>
       <c r="C127" s="2" t="s">
@@ -4295,14 +4166,13 @@
       <c r="G127" s="2">
         <v>113</v>
       </c>
-      <c r="H127" s="4"/>
-    </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128">
         <f t="shared" si="1"/>
         <v>127</v>
       </c>
-      <c r="B128" s="5" t="s">
+      <c r="B128" s="4" t="s">
         <v>68</v>
       </c>
       <c r="C128" s="2" t="s">
@@ -4320,14 +4190,13 @@
       <c r="G128" s="2">
         <v>123</v>
       </c>
-      <c r="H128" s="4"/>
-    </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129">
         <f t="shared" si="1"/>
         <v>128</v>
       </c>
-      <c r="B129" s="5" t="s">
+      <c r="B129" s="4" t="s">
         <v>68</v>
       </c>
       <c r="C129" s="2" t="s">
@@ -4345,14 +4214,13 @@
       <c r="G129" s="2">
         <v>139</v>
       </c>
-      <c r="H129" s="4"/>
-    </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130">
         <f t="shared" si="1"/>
         <v>129</v>
       </c>
-      <c r="B130" s="5" t="s">
+      <c r="B130" s="4" t="s">
         <v>68</v>
       </c>
       <c r="C130" s="2" t="s">
@@ -4370,14 +4238,13 @@
       <c r="G130" s="2">
         <v>111</v>
       </c>
-      <c r="H130" s="4"/>
-    </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131">
         <f t="shared" si="1"/>
         <v>130</v>
       </c>
-      <c r="B131" s="5" t="s">
+      <c r="B131" s="4" t="s">
         <v>68</v>
       </c>
       <c r="C131" s="2" t="s">
@@ -4395,14 +4262,13 @@
       <c r="G131" s="2">
         <v>124</v>
       </c>
-      <c r="H131" s="4"/>
-    </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132">
         <f t="shared" ref="A132:A169" si="2">A131+1</f>
         <v>131</v>
       </c>
-      <c r="B132" s="5" t="s">
+      <c r="B132" s="4" t="s">
         <v>69</v>
       </c>
       <c r="C132" s="2" t="s">
@@ -4420,14 +4286,13 @@
       <c r="G132" s="2">
         <v>119</v>
       </c>
-      <c r="H132" s="4"/>
-    </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133">
         <f t="shared" si="2"/>
         <v>132</v>
       </c>
-      <c r="B133" s="5" t="s">
+      <c r="B133" s="4" t="s">
         <v>69</v>
       </c>
       <c r="C133" s="2" t="s">
@@ -4445,14 +4310,13 @@
       <c r="G133" s="2">
         <v>97</v>
       </c>
-      <c r="H133" s="4"/>
-    </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134">
         <f t="shared" si="2"/>
         <v>133</v>
       </c>
-      <c r="B134" s="5" t="s">
+      <c r="B134" s="4" t="s">
         <v>69</v>
       </c>
       <c r="C134" s="2" t="s">
@@ -4470,14 +4334,13 @@
       <c r="G134" s="2">
         <v>122</v>
       </c>
-      <c r="H134" s="4"/>
-    </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135">
         <f t="shared" si="2"/>
         <v>134</v>
       </c>
-      <c r="B135" s="5" t="s">
+      <c r="B135" s="4" t="s">
         <v>69</v>
       </c>
       <c r="C135" s="2" t="s">
@@ -4495,14 +4358,13 @@
       <c r="G135" s="2">
         <v>115</v>
       </c>
-      <c r="H135" s="4"/>
-    </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136">
         <f t="shared" si="2"/>
         <v>135</v>
       </c>
-      <c r="B136" s="5" t="s">
+      <c r="B136" s="4" t="s">
         <v>69</v>
       </c>
       <c r="C136" s="2" t="s">
@@ -4520,14 +4382,13 @@
       <c r="G136" s="2">
         <v>118</v>
       </c>
-      <c r="H136" s="4"/>
-    </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137">
         <f t="shared" si="2"/>
         <v>136</v>
       </c>
-      <c r="B137" s="5" t="s">
+      <c r="B137" s="4" t="s">
         <v>69</v>
       </c>
       <c r="C137" s="2" t="s">
@@ -4545,14 +4406,13 @@
       <c r="G137" s="2">
         <v>106</v>
       </c>
-      <c r="H137" s="4"/>
-    </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138">
         <f t="shared" si="2"/>
         <v>137</v>
       </c>
-      <c r="B138" s="5" t="s">
+      <c r="B138" s="4" t="s">
         <v>69</v>
       </c>
       <c r="C138" s="2" t="s">
@@ -4570,14 +4430,13 @@
       <c r="G138" s="2">
         <v>94</v>
       </c>
-      <c r="H138" s="4"/>
-    </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139">
         <f t="shared" si="2"/>
         <v>138</v>
       </c>
-      <c r="B139" s="5" t="s">
+      <c r="B139" s="4" t="s">
         <v>70</v>
       </c>
       <c r="C139" s="2" t="s">
@@ -4595,14 +4454,13 @@
       <c r="G139" s="2">
         <v>107</v>
       </c>
-      <c r="H139" s="4"/>
-    </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140">
         <f t="shared" si="2"/>
         <v>139</v>
       </c>
-      <c r="B140" s="5" t="s">
+      <c r="B140" s="4" t="s">
         <v>70</v>
       </c>
       <c r="C140" s="2" t="s">
@@ -4620,14 +4478,13 @@
       <c r="G140" s="2">
         <v>108</v>
       </c>
-      <c r="H140" s="4"/>
-    </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141">
         <f t="shared" si="2"/>
         <v>140</v>
       </c>
-      <c r="B141" s="5" t="s">
+      <c r="B141" s="4" t="s">
         <v>70</v>
       </c>
       <c r="C141" s="2" t="s">
@@ -4645,14 +4502,13 @@
       <c r="G141" s="2">
         <v>110</v>
       </c>
-      <c r="H141" s="4"/>
-    </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142">
         <f t="shared" si="2"/>
         <v>141</v>
       </c>
-      <c r="B142" s="5" t="s">
+      <c r="B142" s="4" t="s">
         <v>70</v>
       </c>
       <c r="C142" s="2" t="s">
@@ -4670,14 +4526,13 @@
       <c r="G142" s="2">
         <v>120</v>
       </c>
-      <c r="H142" s="4"/>
-    </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143">
         <f t="shared" si="2"/>
         <v>142</v>
       </c>
-      <c r="B143" s="5" t="s">
+      <c r="B143" s="4" t="s">
         <v>70</v>
       </c>
       <c r="C143" s="2" t="s">
@@ -4695,14 +4550,13 @@
       <c r="G143" s="2">
         <v>126</v>
       </c>
-      <c r="H143" s="4"/>
-    </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144">
         <f t="shared" si="2"/>
         <v>143</v>
       </c>
-      <c r="B144" s="5" t="s">
+      <c r="B144" s="4" t="s">
         <v>70</v>
       </c>
       <c r="C144" s="2" t="s">
@@ -4720,14 +4574,13 @@
       <c r="G144" s="2">
         <v>140</v>
       </c>
-      <c r="H144" s="4"/>
-    </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145">
         <f t="shared" si="2"/>
         <v>144</v>
       </c>
-      <c r="B145" s="5" t="s">
+      <c r="B145" s="4" t="s">
         <v>70</v>
       </c>
       <c r="C145" s="2" t="s">
@@ -4745,14 +4598,13 @@
       <c r="G145" s="2">
         <v>103</v>
       </c>
-      <c r="H145" s="4"/>
-    </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146">
         <f t="shared" si="2"/>
         <v>145</v>
       </c>
-      <c r="B146" s="5" t="s">
+      <c r="B146" s="4" t="s">
         <v>70</v>
       </c>
       <c r="C146" s="2" t="s">
@@ -4770,14 +4622,13 @@
       <c r="G146" s="2">
         <v>92</v>
       </c>
-      <c r="H146" s="4"/>
-    </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147">
         <f t="shared" si="2"/>
         <v>146</v>
       </c>
-      <c r="B147" s="5" t="s">
+      <c r="B147" s="4" t="s">
         <v>70</v>
       </c>
       <c r="C147" s="2" t="s">
@@ -4795,14 +4646,13 @@
       <c r="G147" s="2">
         <v>103</v>
       </c>
-      <c r="H147" s="4"/>
-    </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148">
         <f t="shared" si="2"/>
         <v>147</v>
       </c>
-      <c r="B148" s="5" t="s">
+      <c r="B148" s="4" t="s">
         <v>71</v>
       </c>
       <c r="C148" s="2" t="s">
@@ -4820,14 +4670,13 @@
       <c r="G148" s="2">
         <v>115</v>
       </c>
-      <c r="H148" s="4"/>
-    </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149">
         <f t="shared" si="2"/>
         <v>148</v>
       </c>
-      <c r="B149" s="5" t="s">
+      <c r="B149" s="4" t="s">
         <v>71</v>
       </c>
       <c r="C149" s="2" t="s">
@@ -4845,14 +4694,13 @@
       <c r="G149" s="2">
         <v>106</v>
       </c>
-      <c r="H149" s="4"/>
-    </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150">
         <f t="shared" si="2"/>
         <v>149</v>
       </c>
-      <c r="B150" s="5" t="s">
+      <c r="B150" s="4" t="s">
         <v>71</v>
       </c>
       <c r="C150" s="2" t="s">
@@ -4870,14 +4718,13 @@
       <c r="G150" s="2">
         <v>112</v>
       </c>
-      <c r="H150" s="4"/>
-    </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151">
         <f t="shared" si="2"/>
         <v>150</v>
       </c>
-      <c r="B151" s="5" t="s">
+      <c r="B151" s="4" t="s">
         <v>71</v>
       </c>
       <c r="C151" s="2" t="s">
@@ -4895,14 +4742,13 @@
       <c r="G151" s="2">
         <v>86</v>
       </c>
-      <c r="H151" s="4"/>
-    </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152">
         <f t="shared" si="2"/>
         <v>151</v>
       </c>
-      <c r="B152" s="5" t="s">
+      <c r="B152" s="4" t="s">
         <v>72</v>
       </c>
       <c r="C152" s="2" t="s">
@@ -4920,14 +4766,13 @@
       <c r="G152" s="2">
         <v>136</v>
       </c>
-      <c r="H152" s="4"/>
-    </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153">
         <f t="shared" si="2"/>
         <v>152</v>
       </c>
-      <c r="B153" s="5" t="s">
+      <c r="B153" s="4" t="s">
         <v>72</v>
       </c>
       <c r="C153" s="2" t="s">
@@ -4945,14 +4790,13 @@
       <c r="G153" s="2">
         <v>141</v>
       </c>
-      <c r="H153" s="4"/>
-    </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154">
         <f t="shared" si="2"/>
         <v>153</v>
       </c>
-      <c r="B154" s="5" t="s">
+      <c r="B154" s="4" t="s">
         <v>72</v>
       </c>
       <c r="C154" s="2" t="s">
@@ -4970,14 +4814,13 @@
       <c r="G154" s="2">
         <v>96</v>
       </c>
-      <c r="H154" s="4"/>
-    </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155">
         <f t="shared" si="2"/>
         <v>154</v>
       </c>
-      <c r="B155" s="5" t="s">
+      <c r="B155" s="4" t="s">
         <v>72</v>
       </c>
       <c r="C155" s="2" t="s">
@@ -4995,14 +4838,13 @@
       <c r="G155" s="2">
         <v>101</v>
       </c>
-      <c r="H155" s="4"/>
-    </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156">
         <f t="shared" si="2"/>
         <v>155</v>
       </c>
-      <c r="B156" s="5" t="s">
+      <c r="B156" s="4" t="s">
         <v>72</v>
       </c>
       <c r="C156" s="2" t="s">
@@ -5020,14 +4862,13 @@
       <c r="G156" s="2">
         <v>126</v>
       </c>
-      <c r="H156" s="4"/>
-    </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157">
         <f t="shared" si="2"/>
         <v>156</v>
       </c>
-      <c r="B157" s="5" t="s">
+      <c r="B157" s="4" t="s">
         <v>72</v>
       </c>
       <c r="C157" s="2" t="s">
@@ -5045,14 +4886,13 @@
       <c r="G157" s="2">
         <v>133</v>
       </c>
-      <c r="H157" s="4"/>
-    </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158">
         <f t="shared" si="2"/>
         <v>157</v>
       </c>
-      <c r="B158" s="5" t="s">
+      <c r="B158" s="4" t="s">
         <v>72</v>
       </c>
       <c r="C158" s="2" t="s">
@@ -5070,14 +4910,13 @@
       <c r="G158" s="2">
         <v>116</v>
       </c>
-      <c r="H158" s="4"/>
-    </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159">
         <f t="shared" si="2"/>
         <v>158</v>
       </c>
-      <c r="B159" s="5" t="s">
+      <c r="B159" s="4" t="s">
         <v>72</v>
       </c>
       <c r="C159" s="2" t="s">
@@ -5095,14 +4934,13 @@
       <c r="G159" s="2">
         <v>111</v>
       </c>
-      <c r="H159" s="4"/>
-    </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160">
         <f t="shared" si="2"/>
         <v>159</v>
       </c>
-      <c r="B160" s="5" t="s">
+      <c r="B160" s="4" t="s">
         <v>72</v>
       </c>
       <c r="C160" s="2" t="s">
@@ -5120,14 +4958,13 @@
       <c r="G160" s="2">
         <v>129</v>
       </c>
-      <c r="H160" s="4"/>
-    </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161">
         <f t="shared" si="2"/>
         <v>160</v>
       </c>
-      <c r="B161" s="5" t="s">
+      <c r="B161" s="4" t="s">
         <v>72</v>
       </c>
       <c r="C161" s="2" t="s">
@@ -5145,14 +4982,13 @@
       <c r="G161" s="2">
         <v>132</v>
       </c>
-      <c r="H161" s="4"/>
-    </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162">
         <f t="shared" si="2"/>
         <v>161</v>
       </c>
-      <c r="B162" s="5" t="s">
+      <c r="B162" s="4" t="s">
         <v>73</v>
       </c>
       <c r="C162" s="2" t="s">
@@ -5170,14 +5006,13 @@
       <c r="G162" s="2">
         <v>125</v>
       </c>
-      <c r="H162" s="4"/>
-    </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163">
         <f t="shared" si="2"/>
         <v>162</v>
       </c>
-      <c r="B163" s="5" t="s">
+      <c r="B163" s="4" t="s">
         <v>73</v>
       </c>
       <c r="C163" s="2" t="s">
@@ -5195,14 +5030,13 @@
       <c r="G163" s="2">
         <v>129</v>
       </c>
-      <c r="H163" s="4"/>
-    </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164">
         <f t="shared" si="2"/>
         <v>163</v>
       </c>
-      <c r="B164" s="5" t="s">
+      <c r="B164" s="4" t="s">
         <v>73</v>
       </c>
       <c r="C164" s="2" t="s">
@@ -5220,14 +5054,13 @@
       <c r="G164" s="2">
         <v>116</v>
       </c>
-      <c r="H164" s="4"/>
-    </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165">
         <f t="shared" si="2"/>
         <v>164</v>
       </c>
-      <c r="B165" s="5" t="s">
+      <c r="B165" s="4" t="s">
         <v>73</v>
       </c>
       <c r="C165" s="2" t="s">
@@ -5245,14 +5078,13 @@
       <c r="G165" s="2">
         <v>104</v>
       </c>
-      <c r="H165" s="4"/>
-    </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166">
         <f t="shared" si="2"/>
         <v>165</v>
       </c>
-      <c r="B166" s="5" t="s">
+      <c r="B166" s="4" t="s">
         <v>73</v>
       </c>
       <c r="C166" s="2" t="s">
@@ -5270,14 +5102,13 @@
       <c r="G166" s="2">
         <v>105</v>
       </c>
-      <c r="H166" s="4"/>
-    </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167">
         <f t="shared" si="2"/>
         <v>166</v>
       </c>
-      <c r="B167" s="5" t="s">
+      <c r="B167" s="4" t="s">
         <v>73</v>
       </c>
       <c r="C167" s="2" t="s">
@@ -5295,14 +5126,13 @@
       <c r="G167" s="2">
         <v>110</v>
       </c>
-      <c r="H167" s="4"/>
-    </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168">
         <f t="shared" si="2"/>
         <v>167</v>
       </c>
-      <c r="B168" s="5" t="s">
+      <c r="B168" s="4" t="s">
         <v>73</v>
       </c>
       <c r="C168" s="2" t="s">
@@ -5320,14 +5150,13 @@
       <c r="G168" s="2">
         <v>114</v>
       </c>
-      <c r="H168" s="4"/>
-    </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169">
         <f t="shared" si="2"/>
         <v>168</v>
       </c>
-      <c r="B169" s="5" t="s">
+      <c r="B169" s="4" t="s">
         <v>73</v>
       </c>
       <c r="C169" s="2" t="s">
@@ -5345,7 +5174,6 @@
       <c r="G169" s="2">
         <v>99</v>
       </c>
-      <c r="H169" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>

</xml_diff>